<commit_message>
updated remaining items doc - added Pat's joystick mapping doc
</commit_message>
<xml_diff>
--- a/RemainingFRC.xlsx
+++ b/RemainingFRC.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RussS9\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitLocalRepos\WM6423_Documents_2019\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{834B31CA-5E11-4B58-A273-8DDD43DB06EB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{923CCF10-9AC1-4405-9FE4-769D0AC2B2E3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8988" xr2:uid="{134CF513-CDC7-4D69-9AC1-FAC1C1AF42B5}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9732" xr2:uid="{134CF513-CDC7-4D69-9AC1-FAC1C1AF42B5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="46">
   <si>
     <t>write</t>
   </si>
@@ -75,27 +75,15 @@
     <t>1st, 2nd robot difference code switches</t>
   </si>
   <si>
-    <t>Trevor,Russ</t>
-  </si>
-  <si>
     <t>task</t>
   </si>
   <si>
-    <t>WM FRC 2019 Software Status - Feb 11, 2019</t>
-  </si>
-  <si>
     <t>status/notes</t>
   </si>
   <si>
-    <t>copy tape state, rename and change to line follower</t>
-  </si>
-  <si>
     <t>assigned to *</t>
   </si>
   <si>
-    <t>Williams, Rogers, Joshua, Trevor, Pat</t>
-  </si>
-  <si>
     <t>lift wheel drop control definition</t>
   </si>
   <si>
@@ -117,30 +105,12 @@
     <t>driver assist control from Pi</t>
   </si>
   <si>
-    <t xml:space="preserve">aquireDisk,  deployDisk, deployBall </t>
-  </si>
-  <si>
     <t>Live feed to driver station</t>
   </si>
   <si>
-    <t>camera; identify, purchase, set up roborio and driver station</t>
-  </si>
-  <si>
-    <t>TBD</t>
-  </si>
-  <si>
-    <t>Russ, TBD</t>
-  </si>
-  <si>
     <t>arm/wrist PID</t>
   </si>
   <si>
-    <t>Trevor,Russ,TBD</t>
-  </si>
-  <si>
-    <t>Trevor, Russ, TBD</t>
-  </si>
-  <si>
     <t>arm/wrist pose data structures  and constants</t>
   </si>
   <si>
@@ -150,22 +120,55 @@
     <t>Russ, Pat</t>
   </si>
   <si>
-    <t>dual driver mode? Reverse drive mode ?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">* identify/assign/setup non-senior developers </t>
-  </si>
-  <si>
-    <t>Joshua</t>
-  </si>
-  <si>
-    <t>setup i3 laptop, vscode, java, git</t>
-  </si>
-  <si>
     <t>program can IDs/map devices</t>
   </si>
   <si>
     <t>teleop and auto periodic</t>
+  </si>
+  <si>
+    <t>Trevor,Russ,Pat</t>
+  </si>
+  <si>
+    <t>Trevor,Pat</t>
+  </si>
+  <si>
+    <t>Trevor, Pat</t>
+  </si>
+  <si>
+    <t>Trevor, Joshua</t>
+  </si>
+  <si>
+    <t>Josha</t>
+  </si>
+  <si>
+    <t>WM FRC 2019 Software Status - Feb 15, 2019</t>
+  </si>
+  <si>
+    <t>waiting for 2nd build to start</t>
+  </si>
+  <si>
+    <t>waiting for diff doc</t>
+  </si>
+  <si>
+    <t>DONE</t>
+  </si>
+  <si>
+    <t>Joshua,Pat, Trevor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">non-senior programmers: identify, train, assign tasks </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ready to start: aquireDisk,  deployDisk, deployBall </t>
+  </si>
+  <si>
+    <t>ready to start</t>
+  </si>
+  <si>
+    <t>ready to start: copy tape state, rename and change to line follower</t>
+  </si>
+  <si>
+    <t>camera; Joshua has two camera samples; need to set up roborio and driver station; work with mechanical team and driver to mount</t>
   </si>
 </sst>
 </file>
@@ -532,10 +535,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42CFA936-5015-4A69-8E08-46342CCB8BE2}">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" zoomScale="137" zoomScaleNormal="137" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -548,89 +551,83 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="F2" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="1">
-        <v>3</v>
-      </c>
-      <c r="C3" s="1">
-        <v>2</v>
-      </c>
-      <c r="D3" s="1">
-        <v>2</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="1">
-        <v>2</v>
-      </c>
-      <c r="C4" s="1">
-        <v>2</v>
-      </c>
-      <c r="D4" s="1">
-        <v>2</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>10</v>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="3">
+        <v>6</v>
+      </c>
+      <c r="C4" s="3">
+        <v>6</v>
+      </c>
+      <c r="D4" s="3">
+        <v>2</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="B5" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C5" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D5" s="1">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="B6" s="1">
         <v>2</v>
@@ -640,6 +637,9 @@
       </c>
       <c r="D6" s="1">
         <v>2</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>44</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>3</v>
@@ -647,53 +647,62 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B7" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C7" s="1">
         <v>2</v>
       </c>
       <c r="D7" s="1">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>43</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B8" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C8" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D8" s="1">
         <v>0</v>
       </c>
+      <c r="E8" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="F8" s="1" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="B9" s="1">
         <v>2</v>
       </c>
       <c r="C9" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D9" s="1">
         <v>0</v>
       </c>
+      <c r="E9" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="F9" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -709,8 +718,11 @@
       <c r="D10" s="1">
         <v>2</v>
       </c>
+      <c r="E10" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="F10" s="1" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -726,8 +738,11 @@
       <c r="D11" s="1">
         <v>0</v>
       </c>
+      <c r="E11" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="F11" s="1" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -743,13 +758,16 @@
       <c r="D12" s="1">
         <v>0</v>
       </c>
+      <c r="E12" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="F12" s="1" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B13" s="1">
         <v>1</v>
@@ -760,13 +778,16 @@
       <c r="D13" s="1">
         <v>0</v>
       </c>
+      <c r="E13" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="F13" s="1" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B14" s="1">
         <v>1</v>
@@ -777,31 +798,37 @@
       <c r="D14" s="1">
         <v>0</v>
       </c>
+      <c r="E14" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="F14" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="1">
+        <v>2</v>
+      </c>
+      <c r="C15" s="1">
+        <v>2</v>
+      </c>
+      <c r="D15" s="1">
+        <v>1</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="1">
-        <v>1</v>
-      </c>
-      <c r="C15" s="1">
-        <v>0</v>
-      </c>
-      <c r="D15" s="1">
-        <v>0</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="B16" s="1">
         <v>2</v>
       </c>
@@ -809,18 +836,15 @@
         <v>2</v>
       </c>
       <c r="D16" s="1">
-        <v>1</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="B17" s="1">
         <v>2</v>
@@ -832,15 +856,15 @@
         <v>2</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>32</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B18" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C18" s="1">
         <v>2</v>
@@ -849,70 +873,66 @@
         <v>2</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B19" s="1">
-        <v>0</v>
-      </c>
-      <c r="C19" s="1">
-        <v>2</v>
-      </c>
-      <c r="D19" s="1">
-        <v>2</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="20" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="21" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="1">
+        <v>1</v>
+      </c>
+      <c r="C21" s="1">
+        <v>0</v>
+      </c>
+      <c r="D21" s="1">
+        <v>0</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" s="1">
+        <v>2</v>
+      </c>
+      <c r="C22" s="1">
+        <v>2</v>
+      </c>
+      <c r="D22" s="1">
+        <v>0</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="F22" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" s="1">
+        <v>1</v>
+      </c>
+      <c r="C23" s="1">
+        <v>0</v>
+      </c>
+      <c r="D23" s="1">
+        <v>0</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F23" s="1" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B22" s="3">
-        <v>6</v>
-      </c>
-      <c r="C22" s="3">
-        <v>6</v>
-      </c>
-      <c r="D22" s="3">
-        <v>2</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="24" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="25" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>